<commit_message>
removed dist and build
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O172"/>
+  <dimension ref="A1:O176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -13330,6 +13330,306 @@
         </is>
       </c>
     </row>
+    <row r="173">
+      <c r="A173" s="2" t="n">
+        <v>172</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O173" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="n">
+        <v>173</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O174" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="n">
+        <v>174</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O175" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="n">
+        <v>175</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O176" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor: add builder class
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O177"/>
+  <dimension ref="A1:O181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -13705,6 +13705,306 @@
         </is>
       </c>
     </row>
+    <row r="178">
+      <c r="A178" s="2" t="n">
+        <v>177</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L178" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M178" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N178" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O178" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="n">
+        <v>178</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O179" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="n">
+        <v>179</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O180" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="n">
+        <v>180</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L181" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M181" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N181" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O181" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: create webservice folder
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O181"/>
+  <dimension ref="A1:O182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -14005,6 +14005,81 @@
         </is>
       </c>
     </row>
+    <row r="182">
+      <c r="A182" s="2" t="n">
+        <v>181</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O182" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: add cs detctor response to page
</commit_message>
<xml_diff>
--- a/communitySmellsDataset.xlsx
+++ b/communitySmellsDataset.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O182"/>
+  <dimension ref="A1:O189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -14080,6 +14080,531 @@
         </is>
       </c>
     </row>
+    <row r="183">
+      <c r="A183" s="2" t="n">
+        <v>182</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L183" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M183" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N183" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O183" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="2" t="n">
+        <v>183</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O184" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="2" t="n">
+        <v>184</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N185" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O185" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="2" t="n">
+        <v>185</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J186" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O186" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="2" t="n">
+        <v>186</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L187" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M187" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N187" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O187" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="2" t="n">
+        <v>187</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L188" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M188" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N188" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O188" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="2" t="n">
+        <v>188</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>https://github.com/ersilia-os/ersilia</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>ersilia</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>ersilia-os</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>07/04/2020</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L189" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M189" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N189" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O189" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>